<commit_message>
Poprawki językowe i aktualizacja wykresów do 4.3 włącznie.
</commit_message>
<xml_diff>
--- a/rysunki/transfery_z_UE.xlsx
+++ b/rysunki/transfery_z_UE.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iwo_a\Documents\MMT_book\rysunki\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iwo.augustynski\Documents\MMT_book\rysunki\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20928" yWindow="1152" windowWidth="27756" windowHeight="14772"/>
+    <workbookView xWindow="-20925" yWindow="1155" windowWidth="27750" windowHeight="14775"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -1869,16 +1869,16 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22:M24"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2004</v>
       </c>
@@ -1918,7 +1918,7 @@
       </c>
       <c r="G2" s="12"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2005</v>
       </c>
@@ -1941,7 +1941,7 @@
       </c>
       <c r="G3" s="13"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2006</v>
       </c>
@@ -1964,7 +1964,7 @@
       </c>
       <c r="G4" s="13"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2007</v>
       </c>
@@ -1987,7 +1987,7 @@
       </c>
       <c r="G5" s="13"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2008</v>
       </c>
@@ -2010,7 +2010,7 @@
       </c>
       <c r="G6" s="13"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2009</v>
       </c>
@@ -2033,7 +2033,7 @@
       </c>
       <c r="G7" s="13"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2010</v>
       </c>
@@ -2056,7 +2056,7 @@
       </c>
       <c r="G8" s="13"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2011</v>
       </c>
@@ -2079,7 +2079,7 @@
       </c>
       <c r="G9" s="12"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2012</v>
       </c>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="G10" s="12"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2013</v>
       </c>
@@ -2125,7 +2125,7 @@
       </c>
       <c r="G11" s="13"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2014</v>
       </c>
@@ -2148,7 +2148,7 @@
       </c>
       <c r="G12" s="13"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2015</v>
       </c>
@@ -2171,7 +2171,7 @@
       </c>
       <c r="G13" s="13"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2016</v>
       </c>
@@ -2194,7 +2194,7 @@
       </c>
       <c r="G14" s="13"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2017</v>
       </c>
@@ -2217,7 +2217,7 @@
       </c>
       <c r="G15" s="13"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2018</v>
       </c>
@@ -2240,7 +2240,7 @@
       </c>
       <c r="G16" s="13"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2019</v>
       </c>
@@ -2263,7 +2263,7 @@
       </c>
       <c r="G17" s="13"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2020</v>
       </c>
@@ -2286,7 +2286,7 @@
       </c>
       <c r="G18" s="13"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2021</v>
       </c>
@@ -2308,7 +2308,29 @@
         <v>105.1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2022</v>
+      </c>
+      <c r="B20" s="1">
+        <v>11265827540</v>
+      </c>
+      <c r="C20" s="14">
+        <v>656905.5</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" ref="D20" si="2">B20/1000000/C20</f>
+        <v>1.7149845053816722E-2</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" ref="E20" si="3">(F20-100)/100</f>
+        <v>0.14400000000000004</v>
+      </c>
+      <c r="F20" s="3">
+        <v>114.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H22" t="s">
         <v>3</v>
       </c>
@@ -2316,7 +2338,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J23" t="s">
         <v>7</v>
       </c>
@@ -2325,7 +2347,7 @@
         <v>2.7449650082115706E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H24" t="s">
         <v>31</v>
       </c>
@@ -2345,22 +2367,22 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="41.6640625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="17.21875" style="5" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="5"/>
+    <col min="1" max="1" width="19.85546875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="41.7109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
@@ -2368,7 +2390,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>11</v>
       </c>
@@ -2389,7 +2411,7 @@
       <c r="N8" s="16"/>
       <c r="O8" s="16"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>13</v>
       </c>
@@ -2397,7 +2419,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>15</v>
       </c>
@@ -2405,27 +2427,27 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C14" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C17" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C18" s="8" t="s">
         <v>21</v>
       </c>
@@ -2439,7 +2461,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>23</v>
       </c>
@@ -2453,7 +2475,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
         <v>27</v>
       </c>

</xml_diff>